<commit_message>
Restore deployed sources and recovered app.html; prepare local rebuild
</commit_message>
<xml_diff>
--- a/labor-timekeeper/exports/2026-01/2026-01-12/Boban_Abbate_2026-01-12.xlsx
+++ b/labor-timekeeper/exports/2026-01/2026-01-12/Boban_Abbate_2026-01-12.xlsx
@@ -5,13 +5,14 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="Weekly Timesheet" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Jason Schema" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -34,7 +35,7 @@
     <t>2026-01-12</t>
   </si>
   <si>
-    <t>Hopkins</t>
+    <t>Tormey</t>
   </si>
   <si>
     <t>Regular</t>
@@ -43,28 +44,25 @@
     <t>2026-01-13</t>
   </si>
   <si>
-    <t>Hunter</t>
+    <t>Corr</t>
   </si>
   <si>
     <t>2026-01-14</t>
   </si>
   <si>
-    <t>Smith</t>
+    <t>Richer</t>
   </si>
   <si>
     <t>2026-01-15</t>
   </si>
   <si>
-    <t>Jackson / Ho</t>
+    <t>Muncey</t>
   </si>
   <si>
     <t>2026-01-16</t>
   </si>
   <si>
-    <t>Campbell</t>
-  </si>
-  <si>
-    <t>OT</t>
+    <t>Watkins</t>
   </si>
   <si>
     <t>SUBTOTAL</t>
@@ -73,10 +71,37 @@
     <t/>
   </si>
   <si>
-    <t>Reg: 40 / OT: 2</t>
+    <t>Reg: 40 / OT: 0</t>
   </si>
   <si>
     <t>Category: HOURLY</t>
+  </si>
+  <si>
+    <t>HOURLY SUBTOTAL</t>
+  </si>
+  <si>
+    <t>ADMIN SUBTOTAL</t>
+  </si>
+  <si>
+    <t>GRAND TOTAL</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Boban Abbate</t>
+  </si>
+  <si>
+    <t>emp_aA-RzZGWVjdtc2P4</t>
+  </si>
+  <si>
+    <t>Seeded sample hours</t>
   </si>
 </sst>
 </file>
@@ -86,7 +111,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -97,8 +122,12 @@
     <font>
       <b/>
     </font>
+    <font>
+      <b/>
+      <color rgb="FF0000"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +144,16 @@
         <fgColor rgb="FFFFE0B0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAF3E0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F8E0"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -128,13 +167,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
@@ -513,7 +558,7 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -522,7 +567,7 @@
         <v>42.5</v>
       </c>
       <c r="F2" s="1">
-        <v>276.25</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -533,7 +578,7 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -542,7 +587,7 @@
         <v>42.5</v>
       </c>
       <c r="F3" s="1">
-        <v>382.5</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -553,7 +598,7 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -562,7 +607,7 @@
         <v>42.5</v>
       </c>
       <c r="F4" s="1">
-        <v>361.25</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -573,7 +618,7 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -582,7 +627,7 @@
         <v>42.5</v>
       </c>
       <c r="F5" s="1">
-        <v>361.25</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -593,7 +638,7 @@
         <v>16</v>
       </c>
       <c r="C6">
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -602,67 +647,303 @@
         <v>42.5</v>
       </c>
       <c r="F6" s="1">
-        <v>318.75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4">
+        <v>40</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="9">
+        <v>1700</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I6"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1">
+        <v>42.5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>340</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1">
+        <v>42.5</v>
+      </c>
+      <c r="G3" s="1">
+        <v>340</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1">
+        <v>42.5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>340</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1">
+        <v>42.5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>340</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1">
         <v>42.5</v>
       </c>
-      <c r="F7" s="1">
-        <v>127.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="4">
-        <v>42</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="5">
-        <v>1827.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>19</v>
+      <c r="G6" s="1">
+        <v>340</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>